<commit_message>
Report: ESAMS completed. Budget monitoring minor fixed.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
@@ -10,77 +10,65 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$8:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$7:$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>MIZUHO BANK, LTD. - MANILA BRANCH</t>
-  </si>
-  <si>
-    <t>25th Floor, The Zuellig Building, Makati Avenue corner Paseo de Roxas, Makati City 1225</t>
-  </si>
-  <si>
-    <t>ATC</t>
-  </si>
-  <si>
-    <t>NATURE OF INCOME PAYMENT</t>
-  </si>
-  <si>
-    <t>RATE OF TAX</t>
-  </si>
-  <si>
-    <t>AMOUNT OF TAX WITHHELD</t>
-  </si>
-  <si>
-    <t>ALPHALIST OF REGULAR SUPPLIERS BY TOP 10,000 PRIVATE CORPORATIONS</t>
-  </si>
-  <si>
-    <t>SEQ.NO.</t>
-  </si>
-  <si>
-    <t>NAME:</t>
-  </si>
-  <si>
-    <t>ADDRESS:</t>
-  </si>
-  <si>
-    <t>TIN:</t>
-  </si>
-  <si>
-    <t>RDO NAME:</t>
-  </si>
-  <si>
-    <t>004-669-467</t>
-  </si>
-  <si>
-    <t>Large Taxpayers Division</t>
-  </si>
-  <si>
-    <t>RDO CODE: 0116</t>
-  </si>
-  <si>
-    <t>TIN NUMBER</t>
-  </si>
-  <si>
-    <t>TAX BASE</t>
-  </si>
-  <si>
-    <t>SUPPLIER'S NAME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>ELECTRONIC SUNDRY ACCOUNT MANAGEMENT SYSTEM (REPORT)</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SEQ NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SETTLEMENT DATE</t>
+  </si>
+  <si>
+    <t>DR AMOUNT</t>
+  </si>
+  <si>
+    <t>CR AMOUNT</t>
+  </si>
+  <si>
+    <t>BALANCE</t>
+  </si>
+  <si>
+    <t>DH</t>
+  </si>
+  <si>
+    <t>APRV</t>
+  </si>
+  <si>
+    <t>MADE</t>
+  </si>
+  <si>
+    <t>REMARKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Account      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Currency     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Name         </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +93,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -178,54 +157,56 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -243,6 +224,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>10026</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>10026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1030029</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17523</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10026" y="10026"/>
+          <a:ext cx="1010478" cy="350397"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,134 +563,132 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="17" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10" style="16" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="I7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="6"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="J7" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="H6" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.17708333333333334" bottom="0.60416666666666663" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.17708333333333334" bottom="0.76041666666666663" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;D &amp;T&amp;CPage &amp;P</oddFooter>
+    <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Report: -Alphalist vendor name sorted. -Esams changed based on the user request.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCDCCB7-758E-4551-8625-160DEB332455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>ELECTRONIC SUNDRY ACCOUNT MANAGEMENT SYSTEM (REPORT)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -59,16 +57,22 @@
   </si>
   <si>
     <t xml:space="preserve">     Name         </t>
+  </si>
+  <si>
+    <t>SUSPENSE PAYMENT / ETC. CONTROL SHEET</t>
+  </si>
+  <si>
+    <t>Form: III-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +102,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -202,6 +212,12 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,7 +259,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -351,6 +373,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -386,6 +425,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -561,7 +617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -586,34 +642,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="A1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="17"/>
@@ -624,8 +680,9 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B4" s="21"/>
       <c r="C4" s="18"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -635,7 +692,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="17"/>
@@ -643,40 +700,43 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
+      <c r="J5" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORT: -ESAMS adjusted based on the user request. included ss, nc entries. -Outstanding advances. same as esams.
Minor modification on Entry_CV_READONLY. txtccytotal class name added to currency field.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCDCCB7-758E-4551-8625-160DEB332455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE722B8-78FE-4A5E-94E1-DD91CF9D0F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -167,27 +167,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -198,9 +177,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -216,14 +192,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,85 +616,85 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10" style="16" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="28.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="J5" s="20" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="J5" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -708,34 +702,34 @@
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="21" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Report (CSV) : Removed Special characters
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_4.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE722B8-78FE-4A5E-94E1-DD91CF9D0F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +25,6 @@
     <t>SEQ NO</t>
   </si>
   <si>
-    <t xml:space="preserve"> SETTLEMENT DATE</t>
-  </si>
-  <si>
     <t>DR AMOUNT</t>
   </si>
   <si>
@@ -63,12 +59,15 @@
   </si>
   <si>
     <t>Form: III-15</t>
+  </si>
+  <si>
+    <t>ENTRY DATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
@@ -192,32 +191,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -367,23 +366,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -419,23 +401,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -611,12 +576,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -636,34 +601,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="A1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="9"/>
@@ -674,7 +639,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="10"/>
@@ -686,7 +651,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="9"/>
@@ -695,42 +660,42 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="J5" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="I7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="19" t="s">
         <v>8</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>